<commit_message>
cleaned code and added comments
</commit_message>
<xml_diff>
--- a/app/static/categorical_to_numeric_representations.xlsx
+++ b/app/static/categorical_to_numeric_representations.xlsx
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="B285" t="n">
-        <v>2435</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="286">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="B286" t="n">
-        <v>6402</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="287">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>1331</v>
+        <v>6726</v>
       </c>
     </row>
     <row r="288">
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>7590</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="289">
@@ -3322,7 +3322,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>4051</v>
+        <v>5022</v>
       </c>
     </row>
     <row r="290">
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>8406</v>
+        <v>7446</v>
       </c>
     </row>
     <row r="291">
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>6107</v>
+        <v>8344</v>
       </c>
     </row>
     <row r="292">
@@ -3352,7 +3352,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>8731</v>
+        <v>6809</v>
       </c>
     </row>
     <row r="293">
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>5357</v>
+        <v>9828</v>
       </c>
     </row>
     <row r="294">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>6900</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="295">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>3201</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="296">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="B296" t="n">
-        <v>6851</v>
+        <v>9537</v>
       </c>
     </row>
     <row r="297">
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>7208</v>
+        <v>8180</v>
       </c>
     </row>
     <row r="298">
@@ -3412,7 +3412,7 @@
         </is>
       </c>
       <c r="B298" t="n">
-        <v>8670</v>
+        <v>6740</v>
       </c>
     </row>
     <row r="299">
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="B299" t="n">
-        <v>2181</v>
+        <v>5121</v>
       </c>
     </row>
     <row r="300">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>5655</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="301">
@@ -3442,7 +3442,7 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>6061</v>
+        <v>7855</v>
       </c>
     </row>
     <row r="302">
@@ -3452,7 +3452,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>3365</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="303">
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>5037</v>
+        <v>8339</v>
       </c>
     </row>
     <row r="304">
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>6303</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="305">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>2366</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="306">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="B306" t="n">
-        <v>6523</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="307">
@@ -3502,7 +3502,7 @@
         </is>
       </c>
       <c r="B307" t="n">
-        <v>8687</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="308">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>9251</v>
+        <v>4832</v>
       </c>
     </row>
     <row r="309">
@@ -3522,7 +3522,7 @@
         </is>
       </c>
       <c r="B309" t="n">
-        <v>4342</v>
+        <v>7298</v>
       </c>
     </row>
     <row r="310">
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="B310" t="n">
-        <v>1024</v>
+        <v>9288</v>
       </c>
     </row>
     <row r="311">
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="B311" t="n">
-        <v>9223</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="312">
@@ -3552,7 +3552,7 @@
         </is>
       </c>
       <c r="B312" t="n">
-        <v>7141</v>
+        <v>1704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>